<commit_message>
Aggiunto riconoscimento componente collimatore
</commit_message>
<xml_diff>
--- a/ESECUTIVI/LP22-315-0.xlsx
+++ b/ESECUTIVI/LP22-315-0.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UTENTI\00.LAVORI IN CORSO\METALTRONICA\22-315-0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Utenti\00.Lavori in corso\METALTRONICA\22-315-0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BADDDC4B-C811-4E99-99F5-020EBFC961D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FFB964-60DA-4A33-8AA4-E1CC027AE9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="22-315-0" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'22-315-0'!$2:$2</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="265">
   <si>
     <t>Pos.</t>
   </si>
@@ -175,9 +176,6 @@
     <t>M:80-C0603C680G5G</t>
   </si>
   <si>
-    <t>C30,C31,C32,C33,C35,C36,C37,C38,C39,C41,C42</t>
-  </si>
-  <si>
     <t>C0603C104K8RACTU</t>
   </si>
   <si>
@@ -559,9 +557,6 @@
     <t>2K2</t>
   </si>
   <si>
-    <t>R18,R30,R33,R34,R37</t>
-  </si>
-  <si>
     <t>1K</t>
   </si>
   <si>
@@ -739,9 +734,6 @@
     <t>SOT223</t>
   </si>
   <si>
-    <t>U9</t>
-  </si>
-  <si>
     <t>Dual Rail to Rail 5VDC General Purpose</t>
   </si>
   <si>
@@ -805,13 +797,34 @@
     <t>LISTA PARTI SCHEDA 22-315-0</t>
   </si>
   <si>
-    <t>DATA 6/2/2023</t>
+    <t>U9,U12</t>
+  </si>
+  <si>
+    <t>R18,R30,R33,R34,R37,R53,R54</t>
+  </si>
+  <si>
+    <t>R51</t>
+  </si>
+  <si>
+    <t>220K</t>
+  </si>
+  <si>
+    <t>R55</t>
+  </si>
+  <si>
+    <t>1K93</t>
+  </si>
+  <si>
+    <t>C30,C31,C32,C33,C35,C36,C37,C38,C39,C41,C42,C47,C49</t>
+  </si>
+  <si>
+    <t>DATA 18/10/2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1709,11 +1722,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,13 +1745,13 @@
   <sheetData>
     <row r="1" spans="1:9" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -2052,10 +2065,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="10">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>50</v>
+        <v>263</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>10</v>
@@ -2064,7 +2077,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>13</v>
@@ -2084,16 +2097,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>53</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>14</v>
@@ -2102,7 +2115,7 @@
         <v>14</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2113,10 +2126,10 @@
         <v>1</v>
       </c>
       <c r="C16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>56</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>57</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>35</v>
@@ -2131,7 +2144,7 @@
         <v>14</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2142,19 +2155,19 @@
         <v>2</v>
       </c>
       <c r="C17" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="E17" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="F17" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="G17" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>14</v>
@@ -2171,21 +2184,21 @@
         <v>2</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="E18" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>66</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2196,25 +2209,25 @@
         <v>2</v>
       </c>
       <c r="C19" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="E19" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="H19" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="H19" s="11" t="s">
-        <v>73</v>
-      </c>
       <c r="I19" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2225,25 +2238,25 @@
         <v>1</v>
       </c>
       <c r="C20" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="G20" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G20" s="11" t="s">
-        <v>77</v>
-      </c>
       <c r="H20" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2254,25 +2267,25 @@
         <v>6</v>
       </c>
       <c r="C21" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="11" t="s">
+      <c r="F21" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="G21" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="G21" s="11" t="s">
-        <v>81</v>
-      </c>
       <c r="H21" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2283,13 +2296,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>83</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>84</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -2304,13 +2317,13 @@
         <v>2</v>
       </c>
       <c r="C23" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="E23" s="11" t="s">
         <v>86</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>87</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -2325,13 +2338,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>90</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
@@ -2346,25 +2359,25 @@
         <v>1</v>
       </c>
       <c r="C25" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="E25" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="F25" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="G25" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="H25" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="H25" s="11" t="s">
-        <v>96</v>
-      </c>
       <c r="I25" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2375,21 +2388,21 @@
         <v>1</v>
       </c>
       <c r="C26" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>98</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>99</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I26" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2400,21 +2413,21 @@
         <v>2</v>
       </c>
       <c r="C27" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="E27" s="11" t="s">
         <v>103</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>104</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2425,21 +2438,21 @@
         <v>1</v>
       </c>
       <c r="C28" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="E28" s="11" t="s">
         <v>107</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>108</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2450,21 +2463,21 @@
         <v>1</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I29" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="I29" s="11" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2475,10 +2488,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>112</v>
       </c>
       <c r="E30" s="12">
         <v>61200621621</v>
@@ -2487,13 +2500,13 @@
         <v>61200621621</v>
       </c>
       <c r="G30" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="H30" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="H30" s="11" t="s">
+      <c r="I30" s="11" t="s">
         <v>114</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2504,21 +2517,21 @@
         <v>1</v>
       </c>
       <c r="C31" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="E31" s="11" t="s">
         <v>117</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>118</v>
       </c>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
       <c r="H31" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2529,25 +2542,25 @@
         <v>1</v>
       </c>
       <c r="C32" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="E32" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="F32" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="G32" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="F32" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="G32" s="11" t="s">
+      <c r="H32" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="H32" s="11" t="s">
-        <v>124</v>
-      </c>
       <c r="I32" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2558,25 +2571,25 @@
         <v>1</v>
       </c>
       <c r="C33" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="E33" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="F33" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="G33" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="H33" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="H33" s="11" t="s">
+      <c r="I33" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="I33" s="11" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2587,23 +2600,23 @@
         <v>1</v>
       </c>
       <c r="C34" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D34" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="E34" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E34" s="11" t="s">
-        <v>134</v>
-      </c>
       <c r="F34" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G34" s="11"/>
       <c r="H34" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2614,22 +2627,22 @@
         <v>2</v>
       </c>
       <c r="C35" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="E35" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="F35" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="G35" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="G35" s="11" t="s">
-        <v>139</v>
-      </c>
       <c r="H35" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I35" s="11" t="s">
         <v>15</v>
@@ -2643,21 +2656,21 @@
         <v>1</v>
       </c>
       <c r="C36" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="E36" s="11" t="s">
         <v>141</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>142</v>
       </c>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2668,25 +2681,25 @@
         <v>5</v>
       </c>
       <c r="C37" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D37" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="E37" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="F37" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G37" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="F37" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="G37" s="11" t="s">
+      <c r="H37" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="H37" s="11" t="s">
+      <c r="I37" s="11" t="s">
         <v>148</v>
-      </c>
-      <c r="I37" s="11" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2697,21 +2710,21 @@
         <v>1</v>
       </c>
       <c r="C38" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D38" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="E38" s="11" t="s">
         <v>151</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>152</v>
       </c>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
       <c r="H38" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="I38" s="11" t="s">
         <v>153</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2722,19 +2735,19 @@
         <v>1</v>
       </c>
       <c r="C39" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D39" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="E39" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="F39" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G39" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="F39" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>158</v>
       </c>
       <c r="H39" s="11" t="s">
         <v>32</v>
@@ -2751,19 +2764,19 @@
         <v>2</v>
       </c>
       <c r="C40" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E40" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="D40" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>160</v>
-      </c>
       <c r="F40" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H40" s="11" t="s">
         <v>32</v>
@@ -2780,19 +2793,19 @@
         <v>6</v>
       </c>
       <c r="C41" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E41" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="D41" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>162</v>
-      </c>
       <c r="F41" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H41" s="11" t="s">
         <v>32</v>
@@ -2809,19 +2822,19 @@
         <v>1</v>
       </c>
       <c r="C42" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E42" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="D42" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>164</v>
-      </c>
       <c r="F42" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H42" s="11" t="s">
         <v>32</v>
@@ -2838,19 +2851,19 @@
         <v>8</v>
       </c>
       <c r="C43" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E43" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="D43" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>166</v>
-      </c>
       <c r="F43" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H43" s="11" t="s">
         <v>32</v>
@@ -2867,19 +2880,19 @@
         <v>1</v>
       </c>
       <c r="C44" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E44" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="D44" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>168</v>
-      </c>
       <c r="F44" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H44" s="11" t="s">
         <v>32</v>
@@ -2896,13 +2909,13 @@
         <v>3</v>
       </c>
       <c r="C45" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="D45" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="E45" s="11" t="s">
         <v>170</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>171</v>
       </c>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
@@ -2917,19 +2930,19 @@
         <v>1</v>
       </c>
       <c r="C46" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="D46" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>173</v>
-      </c>
       <c r="F46" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H46" s="11" t="s">
         <v>32</v>
@@ -2946,19 +2959,19 @@
         <v>2</v>
       </c>
       <c r="C47" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E47" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="D47" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>175</v>
-      </c>
       <c r="F47" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H47" s="11" t="s">
         <v>32</v>
@@ -2975,19 +2988,19 @@
         <v>3</v>
       </c>
       <c r="C48" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E48" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="D48" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>177</v>
-      </c>
       <c r="F48" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H48" s="11" t="s">
         <v>32</v>
@@ -2996,27 +3009,27 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>48</v>
       </c>
       <c r="B49" s="10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>178</v>
+        <v>258</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F49" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H49" s="11" t="s">
         <v>32</v>
@@ -3033,19 +3046,19 @@
         <v>1</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F50" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H50" s="11" t="s">
         <v>32</v>
@@ -3062,19 +3075,19 @@
         <v>1</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F51" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H51" s="11" t="s">
         <v>32</v>
@@ -3091,19 +3104,19 @@
         <v>1</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F52" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H52" s="11" t="s">
         <v>32</v>
@@ -3120,19 +3133,19 @@
         <v>8</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F53" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H53" s="11" t="s">
         <v>32</v>
@@ -3149,19 +3162,19 @@
         <v>2</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F54" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H54" s="11" t="s">
         <v>32</v>
@@ -3178,19 +3191,19 @@
         <v>3</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F55" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H55" s="11" t="s">
         <v>32</v>
@@ -3207,19 +3220,19 @@
         <v>1</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F56" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H56" s="11" t="s">
         <v>32</v>
@@ -3236,362 +3249,418 @@
         <v>1</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>194</v>
+        <v>259</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>195</v>
+        <v>155</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
+        <v>260</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>157</v>
+      </c>
       <c r="H57" s="11" t="s">
-        <v>158</v>
+        <v>32</v>
       </c>
       <c r="I57" s="11" t="s">
-        <v>197</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="9">
-        <v>57</v>
-      </c>
+      <c r="A58" s="9"/>
       <c r="B58" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>198</v>
+        <v>261</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>199</v>
+        <v>155</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>200</v>
+        <v>262</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="G58" s="11"/>
+        <v>32</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>157</v>
+      </c>
       <c r="H58" s="11" t="s">
         <v>32</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>202</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" s="10">
         <v>1</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="F59" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="G59" s="11" t="s">
-        <v>206</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
       <c r="H59" s="11" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="F60" s="11"/>
+        <v>198</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
+      <c r="H60" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I60" s="11" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" s="10">
         <v>1</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="11"/>
+        <v>203</v>
+      </c>
+      <c r="F61" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="H61" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="I61" s="11" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62" s="10">
         <v>1</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="F62" s="11"/>
       <c r="G62" s="11"/>
-      <c r="H62" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="I62" s="11" t="s">
-        <v>218</v>
-      </c>
+      <c r="H62" s="11"/>
+      <c r="I62" s="11"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63" s="10">
         <v>1</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="F63" s="11"/>
       <c r="G63" s="11"/>
-      <c r="H63" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="I63" s="11" t="s">
-        <v>222</v>
-      </c>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" s="10">
         <v>1</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="F64" s="11"/>
       <c r="G64" s="11"/>
       <c r="H64" s="11" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="I64" s="11" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" s="10">
         <v>1</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="F65" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="G65" s="11" t="s">
-        <v>231</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
       <c r="H65" s="11" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="I65" s="11" t="s">
-        <v>115</v>
+        <v>220</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66" s="10">
         <v>1</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="F66" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="G66" s="11" t="s">
-        <v>236</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
       <c r="H66" s="11" t="s">
-        <v>148</v>
+        <v>224</v>
       </c>
       <c r="I66" s="11" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" s="10">
         <v>1</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
+        <v>228</v>
+      </c>
+      <c r="F67" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>229</v>
+      </c>
       <c r="H67" s="11" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="I67" s="11" t="s">
-        <v>241</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
+        <v>66</v>
+      </c>
+      <c r="B68" s="10">
+        <v>1</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="F68" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="H68" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I68" s="11" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="9">
         <v>67</v>
       </c>
-      <c r="B68" s="10">
-        <v>1</v>
-      </c>
-      <c r="C68" s="11" t="s">
+      <c r="B69" s="10">
+        <v>2</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="I69" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="9">
+        <v>68</v>
+      </c>
+      <c r="B70" s="10">
+        <v>1</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="I70" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="D68" s="11" t="s">
+    </row>
+    <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="9">
+        <v>69</v>
+      </c>
+      <c r="B71" s="10">
+        <v>1</v>
+      </c>
+      <c r="C71" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="E68" s="11" t="s">
+      <c r="D71" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="F68" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="I68" s="11" t="s">
+      <c r="E71" s="11" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="9">
-        <v>68</v>
-      </c>
-      <c r="B69" s="10">
-        <v>1</v>
-      </c>
-      <c r="C69" s="11" t="s">
+      <c r="F71" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="G71" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="D69" s="11" t="s">
+      <c r="H71" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="E69" s="11" t="s">
+      <c r="I71" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F69" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="G69" s="11" t="s">
+    </row>
+    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="9">
+        <v>70</v>
+      </c>
+      <c r="B72" s="10">
+        <v>1</v>
+      </c>
+      <c r="C72" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="H69" s="11" t="s">
+      <c r="D72" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="I69" s="11" t="s">
+      <c r="E72" s="11" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="9">
-        <v>69</v>
-      </c>
-      <c r="B70" s="10">
-        <v>1</v>
-      </c>
-      <c r="C70" s="11" t="s">
+      <c r="F72" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="D70" s="11" t="s">
+      <c r="G72" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="E70" s="11" t="s">
+      <c r="H72" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="F70" s="11" t="s">
+      <c r="I72" s="11" t="s">
         <v>255</v>
-      </c>
-      <c r="G70" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="H70" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="I70" s="11" t="s">
-        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -3602,4 +3671,16 @@
     <oddFooter>&amp;L&amp;F&amp;C&amp;D&amp;R&amp;Pdi&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40A90684-FA95-48F0-A4F6-2D5E7289A6D2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modificato C15 da 0nF a 100nF per possibile instabilità Vref opto
</commit_message>
<xml_diff>
--- a/ESECUTIVI/LP22-315-0.xlsx
+++ b/ESECUTIVI/LP22-315-0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Utenti\00.Lavori in corso\METALTRONICA\22-315-0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Documents\Data\Progetti-GIT\HW\PCB-22-315\ESECUTIVI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FFB964-60DA-4A33-8AA4-E1CC027AE9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA9492F-52B3-4A34-9114-50E488CF8170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="22-315-0" sheetId="1" r:id="rId1"/>
@@ -98,9 +98,6 @@
     <t>1uF</t>
   </si>
   <si>
-    <t>C5,C8,C9,C12,C13</t>
-  </si>
-  <si>
     <t>C7</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>220nF</t>
   </si>
   <si>
-    <t>C14,C15</t>
-  </si>
-  <si>
     <t>MLCC, X7R, 50V 0603</t>
   </si>
   <si>
@@ -819,6 +813,12 @@
   </si>
   <si>
     <t>DATA 18/10/2023</t>
+  </si>
+  <si>
+    <t>C5,C8,C9,C12,C13,C15</t>
+  </si>
+  <si>
+    <t>C14</t>
   </si>
 </sst>
 </file>
@@ -1726,7 +1726,7 @@
   <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,13 +1745,13 @@
   <sheetData>
     <row r="1" spans="1:9" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -1884,10 +1884,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>24</v>
+        <v>263</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>10</v>
@@ -1914,13 +1914,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="E8" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
@@ -1935,13 +1935,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
@@ -1953,13 +1953,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>30</v>
+        <v>264</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>21</v>
@@ -1967,7 +1967,7 @@
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>15</v>
@@ -1981,25 +1981,25 @@
         <v>7</v>
       </c>
       <c r="C11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="F11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="G11" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>37</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>14</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2010,25 +2010,25 @@
         <v>1</v>
       </c>
       <c r="C12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="F12" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="G12" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>14</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2039,19 +2039,19 @@
         <v>2</v>
       </c>
       <c r="C13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="F13" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>47</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>49</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>14</v>
@@ -2068,7 +2068,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>10</v>
@@ -2077,7 +2077,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>13</v>
@@ -2097,16 +2097,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>14</v>
@@ -2115,7 +2115,7 @@
         <v>14</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2126,25 +2126,25 @@
         <v>1</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>14</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2155,19 +2155,19 @@
         <v>2</v>
       </c>
       <c r="C17" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="F17" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="G17" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>62</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>14</v>
@@ -2184,21 +2184,21 @@
         <v>2</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>65</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2209,25 +2209,25 @@
         <v>2</v>
       </c>
       <c r="C19" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="H19" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G19" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>72</v>
-      </c>
       <c r="I19" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2238,25 +2238,25 @@
         <v>1</v>
       </c>
       <c r="C20" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="11" t="s">
+      <c r="G20" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>76</v>
-      </c>
       <c r="H20" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2267,25 +2267,25 @@
         <v>6</v>
       </c>
       <c r="C21" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" s="11" t="s">
+      <c r="G21" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>80</v>
-      </c>
       <c r="H21" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2296,13 +2296,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>81</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>83</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -2317,13 +2317,13 @@
         <v>2</v>
       </c>
       <c r="C23" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>84</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>86</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -2338,13 +2338,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>89</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
@@ -2359,25 +2359,25 @@
         <v>1</v>
       </c>
       <c r="C25" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="F25" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="G25" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="H25" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="G25" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>95</v>
-      </c>
       <c r="I25" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2388,21 +2388,21 @@
         <v>1</v>
       </c>
       <c r="C26" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>98</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2413,21 +2413,21 @@
         <v>2</v>
       </c>
       <c r="C27" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>103</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2438,21 +2438,21 @@
         <v>1</v>
       </c>
       <c r="C28" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" s="11" t="s">
         <v>105</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>107</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2463,21 +2463,21 @@
         <v>1</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2488,10 +2488,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E30" s="12">
         <v>61200621621</v>
@@ -2500,13 +2500,13 @@
         <v>61200621621</v>
       </c>
       <c r="G30" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="I30" s="11" t="s">
         <v>112</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2517,21 +2517,21 @@
         <v>1</v>
       </c>
       <c r="C31" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E31" s="11" t="s">
         <v>115</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>117</v>
       </c>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
       <c r="H31" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2542,25 +2542,25 @@
         <v>1</v>
       </c>
       <c r="C32" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E32" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="F32" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G32" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="H32" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="F32" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>123</v>
-      </c>
       <c r="I32" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2571,25 +2571,25 @@
         <v>1</v>
       </c>
       <c r="C33" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E33" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="F33" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="G33" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="H33" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="I33" s="11" t="s">
         <v>128</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="I33" s="11" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2600,23 +2600,23 @@
         <v>1</v>
       </c>
       <c r="C34" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>133</v>
-      </c>
       <c r="F34" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G34" s="11"/>
       <c r="H34" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2627,22 +2627,22 @@
         <v>2</v>
       </c>
       <c r="C35" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="E35" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="F35" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="G35" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="F35" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>138</v>
-      </c>
       <c r="H35" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I35" s="11" t="s">
         <v>15</v>
@@ -2656,21 +2656,21 @@
         <v>1</v>
       </c>
       <c r="C36" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E36" s="11" t="s">
         <v>139</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>141</v>
       </c>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2681,25 +2681,25 @@
         <v>5</v>
       </c>
       <c r="C37" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="F37" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="G37" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="H37" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="F37" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="G37" s="11" t="s">
+      <c r="I37" s="11" t="s">
         <v>146</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="I37" s="11" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2710,21 +2710,21 @@
         <v>1</v>
       </c>
       <c r="C38" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E38" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>151</v>
       </c>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
       <c r="H38" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2735,22 +2735,22 @@
         <v>1</v>
       </c>
       <c r="C39" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E39" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="F39" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G39" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E39" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="F39" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H39" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I39" s="11" t="s">
         <v>15</v>
@@ -2764,22 +2764,22 @@
         <v>2</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D40" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E40" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H40" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I40" s="11" t="s">
         <v>15</v>
@@ -2793,22 +2793,22 @@
         <v>6</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D41" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E41" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H41" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I41" s="11" t="s">
         <v>15</v>
@@ -2822,22 +2822,22 @@
         <v>1</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D42" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E42" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G42" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H42" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I42" s="11" t="s">
         <v>15</v>
@@ -2851,22 +2851,22 @@
         <v>8</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D43" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G43" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E43" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G43" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H43" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I43" s="11" t="s">
         <v>15</v>
@@ -2880,22 +2880,22 @@
         <v>1</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D44" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E44" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G44" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H44" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I44" s="11" t="s">
         <v>15</v>
@@ -2909,13 +2909,13 @@
         <v>3</v>
       </c>
       <c r="C45" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E45" s="11" t="s">
         <v>168</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>170</v>
       </c>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
@@ -2930,22 +2930,22 @@
         <v>1</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D46" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G46" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E46" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H46" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I46" s="11" t="s">
         <v>15</v>
@@ -2959,22 +2959,22 @@
         <v>2</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D47" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G47" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E47" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="F47" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G47" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H47" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I47" s="11" t="s">
         <v>15</v>
@@ -2988,22 +2988,22 @@
         <v>3</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D48" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G48" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E48" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G48" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H48" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I48" s="11" t="s">
         <v>15</v>
@@ -3017,22 +3017,22 @@
         <v>7</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D49" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G49" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E49" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H49" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I49" s="11" t="s">
         <v>15</v>
@@ -3046,22 +3046,22 @@
         <v>1</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D50" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G50" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E50" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H50" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I50" s="11" t="s">
         <v>15</v>
@@ -3075,22 +3075,22 @@
         <v>1</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D51" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G51" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E51" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="F51" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G51" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H51" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I51" s="11" t="s">
         <v>15</v>
@@ -3104,22 +3104,22 @@
         <v>1</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D52" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G52" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E52" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H52" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I52" s="11" t="s">
         <v>15</v>
@@ -3133,22 +3133,22 @@
         <v>8</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D53" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G53" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E53" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="F53" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G53" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H53" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I53" s="11" t="s">
         <v>15</v>
@@ -3162,22 +3162,22 @@
         <v>2</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D54" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G54" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E54" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="F54" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G54" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H54" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I54" s="11" t="s">
         <v>15</v>
@@ -3191,22 +3191,22 @@
         <v>3</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D55" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G55" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E55" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="F55" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G55" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H55" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I55" s="11" t="s">
         <v>15</v>
@@ -3220,22 +3220,22 @@
         <v>1</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D56" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G56" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E56" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="F56" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G56" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H56" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I56" s="11" t="s">
         <v>15</v>
@@ -3249,22 +3249,22 @@
         <v>1</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D57" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G57" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E57" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="F57" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G57" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H57" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I57" s="11" t="s">
         <v>15</v>
@@ -3276,22 +3276,22 @@
         <v>1</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D58" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G58" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="E58" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="F58" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G58" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="H58" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I58" s="11" t="s">
         <v>15</v>
@@ -3305,21 +3305,21 @@
         <v>1</v>
       </c>
       <c r="C59" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E59" s="11" t="s">
         <v>192</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="E59" s="11" t="s">
-        <v>194</v>
       </c>
       <c r="F59" s="11"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3330,23 +3330,23 @@
         <v>2</v>
       </c>
       <c r="C60" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="E60" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="D60" s="11" t="s">
+      <c r="F60" s="11" t="s">
         <v>197</v>
-      </c>
-      <c r="E60" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="F60" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="G60" s="11"/>
       <c r="H60" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I60" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3357,25 +3357,25 @@
         <v>1</v>
       </c>
       <c r="C61" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="E61" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="D61" s="11" t="s">
+      <c r="F61" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="G61" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="E61" s="11" t="s">
+      <c r="H61" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="F61" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="G61" s="11" t="s">
+      <c r="I61" s="11" t="s">
         <v>204</v>
-      </c>
-      <c r="H61" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="I61" s="11" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3386,13 +3386,13 @@
         <v>1</v>
       </c>
       <c r="C62" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="E62" s="11" t="s">
         <v>207</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="E62" s="11" t="s">
-        <v>209</v>
       </c>
       <c r="F62" s="11"/>
       <c r="G62" s="11"/>
@@ -3407,13 +3407,13 @@
         <v>1</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F63" s="11"/>
       <c r="G63" s="11"/>
@@ -3428,21 +3428,21 @@
         <v>1</v>
       </c>
       <c r="C64" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="E64" s="11" t="s">
         <v>212</v>
-      </c>
-      <c r="D64" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>214</v>
       </c>
       <c r="F64" s="11"/>
       <c r="G64" s="11"/>
       <c r="H64" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I64" s="11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3453,21 +3453,21 @@
         <v>1</v>
       </c>
       <c r="C65" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="E65" s="11" t="s">
         <v>217</v>
-      </c>
-      <c r="D65" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="E65" s="11" t="s">
-        <v>219</v>
       </c>
       <c r="F65" s="11"/>
       <c r="G65" s="11"/>
       <c r="H65" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I65" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3478,21 +3478,21 @@
         <v>1</v>
       </c>
       <c r="C66" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="E66" s="11" t="s">
         <v>221</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="E66" s="11" t="s">
-        <v>223</v>
       </c>
       <c r="F66" s="11"/>
       <c r="G66" s="11"/>
       <c r="H66" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I66" s="11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3503,25 +3503,25 @@
         <v>1</v>
       </c>
       <c r="C67" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E67" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="D67" s="11" t="s">
+      <c r="F67" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="G67" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="E67" s="11" t="s">
+      <c r="H67" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F67" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G67" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="H67" s="11" t="s">
-        <v>230</v>
-      </c>
       <c r="I67" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3532,25 +3532,25 @@
         <v>1</v>
       </c>
       <c r="C68" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E68" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="D68" s="11" t="s">
+      <c r="F68" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="G68" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="E68" s="11" t="s">
+      <c r="H68" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="I68" s="11" t="s">
         <v>233</v>
-      </c>
-      <c r="F68" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="G68" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="H68" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="I68" s="11" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3561,21 +3561,21 @@
         <v>2</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F69" s="11"/>
       <c r="G69" s="11"/>
       <c r="H69" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I69" s="11" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3586,23 +3586,23 @@
         <v>1</v>
       </c>
       <c r="C70" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="E70" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="D70" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="E70" s="11" t="s">
-        <v>241</v>
-      </c>
       <c r="F70" s="11" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G70" s="11"/>
       <c r="H70" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I70" s="11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3613,25 +3613,25 @@
         <v>1</v>
       </c>
       <c r="C71" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="E71" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="D71" s="11" t="s">
+      <c r="F71" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="G71" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="E71" s="11" t="s">
+      <c r="H71" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="F71" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="G71" s="11" t="s">
+      <c r="I71" s="11" t="s">
         <v>246</v>
-      </c>
-      <c r="H71" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="I71" s="11" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3642,25 +3642,25 @@
         <v>1</v>
       </c>
       <c r="C72" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="E72" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="D72" s="11" t="s">
+      <c r="F72" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="E72" s="11" t="s">
+      <c r="G72" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="F72" s="11" t="s">
+      <c r="H72" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="G72" s="11" t="s">
+      <c r="I72" s="11" t="s">
         <v>253</v>
-      </c>
-      <c r="H72" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="I72" s="11" t="s">
-        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>